<commit_message>
Adding comment for power result in python
</commit_message>
<xml_diff>
--- a/Results/Report.xlsx
+++ b/Results/Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\47939\Desktop\Interviews\KTP\Technical_Task _KTP\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F5F80-7FEB-414D-AAA6-F715A7A7565E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E106A7F-97F3-4214-87D6-42346FB03877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{DEF1C0BC-912F-4C98-AC38-2838403C81A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{DEF1C0BC-912F-4C98-AC38-2838403C81A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Network_X_Y" sheetId="3" r:id="rId1"/>
@@ -439,16 +439,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>299223</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>2210</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>159895</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>192114</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>141992</xdr:rowOff>
+      <xdr:colOff>184494</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>57890</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -471,8 +471,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8841243" y="5260010"/>
-          <a:ext cx="2940891" cy="2454032"/>
+          <a:off x="8092315" y="5082540"/>
+          <a:ext cx="3682199" cy="3075410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2801,7 +2801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4177B735-6C8B-4ABD-AACF-3AC5E045D9D3}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
@@ -3819,7 +3819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B627F5E8-98BE-48D3-86B1-8A096C36C42B}">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
@@ -4846,7 +4846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1355452-5ED3-4F6E-8164-D4A90D12F639}">
   <dimension ref="A18:W72"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <selection activeCell="U88" sqref="U88"/>
     </sheetView>
   </sheetViews>

</xml_diff>